<commit_message>
updated ltcf comprehensive list with new LTCFs
</commit_message>
<xml_diff>
--- a/app/shiny/templates/template_order_1211.xlsx
+++ b/app/shiny/templates/template_order_1211.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahu.PH\Documents\GitHub\ppe_allocatoR\app\shiny\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91E1F4A9-478F-4B1C-BBA2-D85F2C0A56FC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4019F505-5265-4BC9-AD3C-B7BD967A074C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{6E043744-41BF-4309-8E15-A193B86EE1CB}"/>
+    <workbookView xWindow="-5040" yWindow="2625" windowWidth="9600" windowHeight="4905" xr2:uid="{6E043744-41BF-4309-8E15-A193B86EE1CB}"/>
   </bookViews>
   <sheets>
     <sheet name="Elections" sheetId="2" r:id="rId1"/>
@@ -162,6 +162,61 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2949575</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>15875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>187325</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>29869</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8C906A93-E1FB-4606-8E2C-AF89FC13ADE2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4454525" y="15875"/>
+          <a:ext cx="2019300" cy="1280819"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -464,7 +519,7 @@
   <dimension ref="A10:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -522,25 +577,11 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009BC94ECF313B5246868E87E2CCF9F2B6" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e7068939f287d0aae6c00b0eaae34d33">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="56db134c-4247-493d-bb73-9f73b9a5dc87" xmlns:ns4="4ad208af-66fe-4634-859b-5e98ffd8fb32" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7f53fc25a8bec057ac1c909ff733d8cc" ns3:_="" ns4:_="">
     <xsd:import namespace="56db134c-4247-493d-bb73-9f73b9a5dc87"/>
@@ -743,32 +784,22 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BF527F85-80F7-456C-8479-F80AEA6BE54F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E9EEBB62-783A-409C-8343-E456CF454898}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="56db134c-4247-493d-bb73-9f73b9a5dc87"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="4ad208af-66fe-4634-859b-5e98ffd8fb32"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3A709E95-7685-4A29-83B9-D8A0640CE435}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -785,4 +816,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E9EEBB62-783A-409C-8343-E456CF454898}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="56db134c-4247-493d-bb73-9f73b9a5dc87"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="4ad208af-66fe-4634-859b-5e98ffd8fb32"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BF527F85-80F7-456C-8479-F80AEA6BE54F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>